<commit_message>
Added excel file hopefully for sure this time
</commit_message>
<xml_diff>
--- a/test_cases.xlsx
+++ b/test_cases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zee/development/CS151_labs/Lab2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\timeg_5sap6w9\PycharmProjects\cs151-lab2-laure-and-owen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C084CA8B-2F93-D948-9FA4-65E66A2852B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{195C0526-B05C-4B1E-BBD0-26F200E68942}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="67920" windowHeight="28300" xr2:uid="{078FF010-DC04-EB46-847F-52BBCCEEE85C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{078FF010-DC04-EB46-847F-52BBCCEEE85C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -164,14 +164,14 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -197,9 +197,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -237,7 +237,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -343,7 +343,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -485,7 +485,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -496,59 +496,60 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:I10"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="38" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.83203125" customWidth="1"/>
-    <col min="3" max="3" width="11.1640625" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" customWidth="1"/>
-    <col min="5" max="5" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.796875" customWidth="1"/>
+    <col min="3" max="3" width="11.19921875" customWidth="1"/>
+    <col min="4" max="4" width="11.296875" customWidth="1"/>
+    <col min="5" max="5" width="26.296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="1">
         <f>60*60*24*365</f>
         <v>31536000</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
@@ -563,99 +564,194 @@
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
     </row>
-    <row r="5" spans="1:9" ht="76" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:9" ht="55.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="I5" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+      <c r="B6" s="1">
+        <v>8</v>
+      </c>
+      <c r="C6" s="1">
+        <v>12</v>
+      </c>
+      <c r="D6" s="1">
+        <v>126</v>
+      </c>
+      <c r="E6" s="1">
+        <v>3331000360</v>
+      </c>
+      <c r="F6" s="1">
+        <v>5</v>
+      </c>
+      <c r="G6" s="1">
+        <f>($B$2/B6+$B$2/D6-$B$2/C6)*F6</f>
+        <v>7821428.5714285709</v>
+      </c>
+      <c r="H6" s="1">
+        <f>G6+E6</f>
+        <v>3338821788.5714288</v>
+      </c>
+      <c r="I6" s="1" t="str">
+        <f>IF(H6&gt;E6, "Increase", "Decrease")</f>
+        <v>Increase</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+      <c r="B7" s="1">
+        <v>2</v>
+      </c>
+      <c r="C7" s="1">
+        <v>12</v>
+      </c>
+      <c r="D7" s="1">
+        <v>126</v>
+      </c>
+      <c r="E7" s="1">
+        <v>3331000360</v>
+      </c>
+      <c r="F7" s="1">
+        <v>5</v>
+      </c>
+      <c r="G7" s="1">
+        <f t="shared" ref="G7:G10" si="0">($B$2/B7+$B$2/D7-$B$2/C7)*F7</f>
+        <v>66951428.571428575</v>
+      </c>
+      <c r="H7" s="1">
+        <f t="shared" ref="H7:H10" si="1">G7+E7</f>
+        <v>3397951788.5714288</v>
+      </c>
+      <c r="I7" s="1" t="str">
+        <f t="shared" ref="I7:I10" si="2">IF(H7&gt;E7, "Increase", "Decrease")</f>
+        <v>Increase</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+      <c r="B8" s="1">
+        <v>8</v>
+      </c>
+      <c r="C8" s="1">
+        <v>12</v>
+      </c>
+      <c r="D8" s="1">
+        <v>2</v>
+      </c>
+      <c r="E8" s="1">
+        <v>3331000360</v>
+      </c>
+      <c r="F8" s="1">
+        <v>5</v>
+      </c>
+      <c r="G8" s="1">
+        <f t="shared" si="0"/>
+        <v>85410000</v>
+      </c>
+      <c r="H8" s="1">
+        <f t="shared" si="1"/>
+        <v>3416410360</v>
+      </c>
+      <c r="I8" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>Increase</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+      <c r="B9" s="1">
+        <v>8</v>
+      </c>
+      <c r="C9" s="1">
+        <v>2</v>
+      </c>
+      <c r="D9" s="1">
+        <v>126</v>
+      </c>
+      <c r="E9" s="1">
+        <v>3331000360</v>
+      </c>
+      <c r="F9" s="1">
+        <v>5</v>
+      </c>
+      <c r="G9" s="1">
+        <f t="shared" si="0"/>
+        <v>-57878571.428571425</v>
+      </c>
+      <c r="H9" s="1">
+        <f t="shared" si="1"/>
+        <v>3273121788.5714288</v>
+      </c>
+      <c r="I9" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>Decrease</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
+      <c r="B10" s="1">
+        <v>50</v>
+      </c>
+      <c r="C10" s="1">
+        <v>12</v>
+      </c>
+      <c r="D10" s="1">
+        <v>200</v>
+      </c>
+      <c r="E10" s="1">
+        <v>3331000360</v>
+      </c>
+      <c r="F10" s="1">
+        <v>5</v>
+      </c>
+      <c r="G10" s="1">
+        <f t="shared" si="0"/>
+        <v>-9198000</v>
+      </c>
+      <c r="H10" s="1">
+        <f t="shared" si="1"/>
+        <v>3321802360</v>
+      </c>
+      <c r="I10" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>Decrease</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>